<commit_message>
send feedback email working fine
</commit_message>
<xml_diff>
--- a/mybaby/src/com/mybaby/feeder/appointments/howtodoinjava_demo.xlsx
+++ b/mybaby/src/com/mybaby/feeder/appointments/howtodoinjava_demo.xlsx
@@ -5,19 +5,22 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Employee Data" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="sms" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="domains" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="todo" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="git" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="kooldoctorzz email" sheetId="6" state="visible" r:id="rId7"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="96">
   <si>
     <t>ID</t>
   </si>
@@ -58,19 +61,50 @@
     <t>Kiran</t>
   </si>
   <si>
-    <t>patientConnect</t>
-  </si>
-  <si>
-    <t>After the visits send sms asking he is feeling better. If not or need any assistance call me on xxxxx</t>
+    <t>Features</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Monetisation</t>
+  </si>
+  <si>
+    <t>patientReconnect</t>
+  </si>
+  <si>
+    <t>After the visits send sms asking he is feeling better or if patient needs any assitance. Patient send a email describing is health condition. May attach images or videos of the patient which help doctor better understand his/her condition. Application reads all these emails and constructs
+A dashboard which lists all the patiants response along with the images/videos. Doctor can go through these respones and chose to respond to them in the following way:
+1. call patient to talk to better understand and assit the patient.
+2. send email/sms what next steps to be take or asking patient to come and visit him.</t>
+  </si>
+  <si>
+    <t>While  generating the invoice for the visit, patient will be prompted to check if he/she needs PatientReconnect feature and a nominal fee will be charged.</t>
   </si>
   <si>
     <t>appointment remainder</t>
   </si>
   <si>
-    <t>send remainder before 1 day about the appointment. This should be configurable.</t>
-  </si>
-  <si>
-    <t>rating the doctor.</t>
+    <t>send remainder before 1 day about the appointment. This should be configurable. Patient responds to the email/sms whether he is coming or not coming or wants to postpone the appointment. Application reads these responses and construct the dash board clasifying the reponses as coming, not coming and need new appointment. A message, email/sms, will be sent with the current status of the appointments</t>
+  </si>
+  <si>
+    <t>Doctors can be charged for this features. This in turn increase doctors revenue. </t>
+  </si>
+  <si>
+    <t>rating the doctor (and its uses) ( Java method name is </t>
+  </si>
+  <si>
+    <t>After the treament send sms/email to the patient asking how they are feeling and asking them to rate the doctor clicking on the rating options in the mailbody itself (Application page is embded in the email body). Application reads these ratings and top rated docs in the locality will be displayed when users search for top rated docs in the locality. By default app shows top rated docs of the patient's locations. Suppose a patient from bangalore searches toprated docs then in bangalore who are the top rated doctrs will be shown. If user searches by top rated docs in India, app displays the docs who are toprated in India. This application also has the feature for anybody to go and rate the doctors directly going to the app. Necessary measures will be taken to avoid unethical rating by humans or by programs (robos).
+Book top rated doc: this application will have the option to book an appointment with the top rated doc. Once patient books an appointment an email/sms will be sent to doc indicating the same. Doctor provides the list of slots per day and are stored in the system. Doctor can see his appointments going to the application also he gets an email/sms daily about the next day's and current day's appointments.</t>
+  </si>
+  <si>
+    <t>doctors can be charged for this features and also taken a cut from the doctors on appointment booking after realization of the appointment.</t>
+  </si>
+  <si>
+    <t>End result is huge data of doctors and patients. Will think over how to use this data for further monetization. 
+For Patients: continuous support of doctors during the treatment. This can also help in uncessary travel to hospital.
+For the Doctor: Promotion through ratings, visiblity via search and online booking.
+</t>
   </si>
   <si>
     <t>messagebird.com</t>
@@ -244,7 +278,34 @@
     <t>kooldoctorz/Mybabyat123</t>
   </si>
   <si>
-    <t>Amazon creds</t>
+    <t>Saturday night</t>
+  </si>
+  <si>
+    <t>insert the date </t>
+  </si>
+  <si>
+    <t>play around calendar object and see how to capture day and time.</t>
+  </si>
+  <si>
+    <t>remainder email</t>
+  </si>
+  <si>
+    <t>if data of next appointment is current date=1 day then remainder emails. So write a query to get all the appoitments whose next appointment is current date+1. </t>
+  </si>
+  <si>
+    <t>reconnect</t>
+  </si>
+  <si>
+    <t>After 2 days of visit and less than next visit check how patient is feeling.</t>
+  </si>
+  <si>
+    <t>feedback</t>
+  </si>
+  <si>
+    <t>after the treatment ask for feedback. How do u decide treatment is over?</t>
+  </si>
+  <si>
+    <t>git</t>
   </si>
   <si>
     <r>
@@ -257,6 +318,23 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
+      <t xml:space="preserve">com/Mybaby@143</t>
+    </r>
+  </si>
+  <si>
+    <t>https://github.com/fazilkarni/mybaby.git</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">kooldoctorzz@gmail.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
       <t xml:space="preserve">com/Fm@Mybaby143</t>
     </r>
   </si>
@@ -268,7 +346,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -288,6 +366,12 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -375,32 +459,44 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -483,25 +579,27 @@
   </sheetPr>
   <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A22" activeCellId="0" sqref="A22"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="46.6785714285714"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="81.8775510204082"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="10.7551020408163"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="81.8775510204082"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="23.1989795918367"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.265306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="10.7551020408163"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
@@ -509,10 +607,10 @@
       <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -520,10 +618,10 @@
       <c r="A3" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="1" t="s">
         <v>6</v>
       </c>
     </row>
@@ -531,10 +629,10 @@
       <c r="A4" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="1" t="s">
         <v>8</v>
       </c>
     </row>
@@ -542,10 +640,10 @@
       <c r="A5" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="1" t="s">
         <v>10</v>
       </c>
     </row>
@@ -553,91 +651,117 @@
       <c r="A6" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" s="1" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="8" s="2" customFormat="true" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
+      </c>
+      <c r="C9" s="0"/>
+    </row>
+    <row r="10" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="0" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="73.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="0" t="s">
-        <v>14</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="191.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C15" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B18" s="0" t="s">
-        <v>20</v>
+      <c r="A18" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="B20" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>24</v>
+        <v>30</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="B21" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>27</v>
+        <v>33</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C22" s="2" t="s">
-        <v>28</v>
+      <c r="C22" s="5" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C23" s="2" t="s">
-        <v>29</v>
+      <c r="C23" s="5" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -661,8 +785,8 @@
   </sheetPr>
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -674,33 +798,33 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>36</v>
+        <v>43</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>44</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>9880396688</v>
@@ -708,10 +832,10 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>38</v>
+        <v>45</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>46</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>9844118651</v>
@@ -719,18 +843,18 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>40</v>
+        <v>47</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>48</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>9663550135</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="1" t="s">
-        <v>41</v>
+      <c r="A22" s="4" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -741,11 +865,11 @@
     <hyperlink ref="A22" r:id="rId4" display="https://2factor.in/CP/register.php"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -755,189 +879,325 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C31"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B32" activeCellId="0" sqref="B32"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B26" activeCellId="0" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.3622448979592"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.8724489795918"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.7602040816327"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.780612244898"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>46</v>
+        <v>53</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="3" t="s">
-        <v>56</v>
+      <c r="A14" s="6" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>58</v>
+        <v>65</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>66</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="4" t="s">
-        <v>61</v>
+      <c r="A17" s="7" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="5" t="s">
-        <v>62</v>
+      <c r="A18" s="8" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="6" t="s">
-        <v>64</v>
+      <c r="A23" s="9" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="2" t="s">
-        <v>65</v>
+      <c r="A24" s="5" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="2" t="s">
-        <v>66</v>
+      <c r="A25" s="5" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="B31" s="0" t="s">
-        <v>76</v>
+        <v>82</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.3520408163265"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="129.122448979592"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>91</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="31.1632653061224"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="33.2448979591837"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B31" r:id="rId1" display="com/Fm@Mybaby143"/>
+    <hyperlink ref="B1" r:id="rId1" display="com/Mybaby@143"/>
+    <hyperlink ref="C1" r:id="rId2" display="https://github.com/fazilkarni/mybaby.git"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.3061224489796"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>95</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1" display="com/Fm@Mybaby143"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>